<commit_message>
I just lost my doooog
</commit_message>
<xml_diff>
--- a/Szabdan/Szoftver teszt/Gyakorlat/Program1/ML-Tesztesetek.xlsx
+++ b/Szabdan/Szoftver teszt/Gyakorlat/Program1/ML-Tesztesetek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\.School\2024-25\Szabdan\Szoftver teszt\Gyakorlat\Program1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\!2024-25\Szabdan\Szoftver teszt\Gyakorlat\Program1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801BCDBA-F074-48D3-98FD-FF72D00C567C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86AACD5-FE5B-4FC3-B1C7-9959288F5F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{E76C08E6-68FF-49AA-88B9-EE0AC9DA6B96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E76C08E6-68FF-49AA-88B9-EE0AC9DA6B96}"/>
   </bookViews>
   <sheets>
     <sheet name="program1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>ADFGVX kódolásnál ha nem adunk meg kulcsszót akkor összeomlik a program</t>
   </si>
   <si>
-    <t>A XOR használatánál nincs kódolásra/dekódolást kiválaszto rádiogomb</t>
-  </si>
-  <si>
     <t>Ha nem olvastál be, is lehet használni a "Beolvasás törlése" gombot</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Sortörés vizsgálata</t>
   </si>
   <si>
-    <t>Ha ékezetes betüket akarsz kódolni, akkor eggyes kódolási metodusok nem támogatják egyesek rosszul kódolják</t>
-  </si>
-  <si>
     <t>Leet kódolás beolvasott fájlal</t>
   </si>
   <si>
@@ -261,10 +255,16 @@
     <t>Összes kódolás/dekódolás</t>
   </si>
   <si>
-    <t>Nem jelez vissza hogy sikerült-e le kódolni</t>
-  </si>
-  <si>
     <t>Leet dekódolása beolvasott fájlal</t>
+  </si>
+  <si>
+    <t>Ha ékezetes betüket akarsz kódolni, akkor eggyes kódolási metodusok nem támogatják, rosszul kódolják</t>
+  </si>
+  <si>
+    <t>Nem jelez vissza hogy sikerült-e le (de)kódolni</t>
+  </si>
+  <si>
+    <t>A XOR használatánál nincs kódolásra/dekódolást kiválasztó gomb</t>
   </si>
 </sst>
 </file>
@@ -317,7 +317,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -333,7 +333,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -651,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0231CE-89BE-4B9A-B007-29C9D24325B8}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -697,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -711,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -725,7 +725,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -739,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -753,10 +753,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -767,10 +767,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
@@ -781,7 +781,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -795,7 +795,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -851,10 +851,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
@@ -879,7 +879,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -896,7 +896,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -935,7 +935,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>22</v>
@@ -963,13 +963,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -977,13 +977,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,10 +994,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1005,13 +1005,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1019,13 +1019,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1033,13 +1033,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1047,13 +1047,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1061,13 +1061,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,13 +1075,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1089,13 +1089,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C129132E-D5C9-42AC-BCD9-E2627BC4C341}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1145,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1161,10 +1161,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1193,7 +1193,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>